<commit_message>
Replace Grid library with Tabular gem
</commit_message>
<xml_diff>
--- a/test/fixtures/results/times.xlsx
+++ b/test/fixtures/results/times.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="0" windowWidth="20160" windowHeight="14380"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Place</t>
   </si>
@@ -157,17 +157,21 @@
   <si>
     <t>Oscar</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Ivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="m:ss.00"/>
-    <numFmt numFmtId="173" formatCode="mm:ss.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="m:ss.00"/>
+    <numFmt numFmtId="165" formatCode="mm:ss.000"/>
+    <numFmt numFmtId="166" formatCode="hh:mm:ss.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -184,6 +188,11 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,11 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="46" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -235,8 +244,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -911,7 +923,15 @@
         <v>44</v>
       </c>
       <c r="F21" s="14">
-        <v>0.41666574074074075</v>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15">
+      <c r="C22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="15">
+        <v>38851.012572106483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>